<commit_message>
local updates on updating ontology to differentiate between protein clusters
</commit_message>
<xml_diff>
--- a/data/targets.xlsx
+++ b/data/targets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/hanmar_dtu_dk/Documents/repos/panRes/ontology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1761" documentId="8_{64C500C0-3572-8C45-8159-DFC9F6BA92DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED83563F-5EDE-6B41-B22D-22963C111318}"/>
+  <xr:revisionPtr revIDLastSave="1868" documentId="8_{64C500C0-3572-8C45-8159-DFC9F6BA92DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8984FD4D-D694-E140-9BAE-80560040DEF9}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{FF6830B3-738E-CB47-A3EA-D65538A3CCFD}"/>
+    <workbookView xWindow="2320" yWindow="2560" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{FF6830B3-738E-CB47-A3EA-D65538A3CCFD}"/>
   </bookViews>
   <sheets>
     <sheet name="antibiotic" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="818">
   <si>
     <t>group</t>
   </si>
@@ -2443,16 +2443,58 @@
     <t>Target protection</t>
   </si>
   <si>
+    <t>Increased efflux</t>
+  </si>
+  <si>
+    <t>Alternate pathway</t>
+  </si>
+  <si>
+    <t>Antibiotic Inactivation</t>
+  </si>
+  <si>
+    <t>Antibiotic Target Replacement</t>
+  </si>
+  <si>
+    <t>Antibiotic Efflux</t>
+  </si>
+  <si>
+    <t>Antibiotic Target Protection</t>
+  </si>
+  <si>
+    <t>Antibiotic Target Alteration</t>
+  </si>
+  <si>
+    <t>Equivalent to</t>
+  </si>
+  <si>
+    <t>Enzymatic Inactivation</t>
+  </si>
+  <si>
+    <t>Ribosylation</t>
+  </si>
+  <si>
+    <t>Reduced Permeability To Antibiotic</t>
+  </si>
+  <si>
+    <t>Resistance by absence</t>
+  </si>
+  <si>
+    <t>Modification to cell morphology</t>
+  </si>
+  <si>
+    <t>Resistance by host-dependent nutrient acquisition</t>
+  </si>
+  <si>
+    <t>Antibiotic target overexpression</t>
+  </si>
+  <si>
+    <t>Isoleucyl tRNA synthetase</t>
+  </si>
+  <si>
     <t>Enzymatic inactivation</t>
   </si>
   <si>
-    <t>Increased efflux</t>
-  </si>
-  <si>
-    <t>Alternate pathway</t>
-  </si>
-  <si>
-    <t>Ribosulation</t>
+    <t>Target Protection</t>
   </si>
 </sst>
 </file>
@@ -3001,6 +3043,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5940E992-45D7-D44C-A2E9-310383C77A27}" name="Table1" displayName="Table1" ref="A1:E274" totalsRowShown="0" dataDxfId="38">
   <autoFilter ref="A1:E274" xr:uid="{5940E992-45D7-D44C-A2E9-310383C77A27}"/>
@@ -3019,13 +3065,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E4D6091A-7BFC-A642-AD14-7BF64597F886}" name="Table7" displayName="Table7" ref="A1:A10" totalsRowShown="0">
-  <autoFilter ref="A1:A10" xr:uid="{E4D6091A-7BFC-A642-AD14-7BF64597F886}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A10">
-    <sortCondition ref="A1:A10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E4D6091A-7BFC-A642-AD14-7BF64597F886}" name="Table7" displayName="Table7" ref="A1:B21" totalsRowShown="0">
+  <autoFilter ref="A1:B21" xr:uid="{E4D6091A-7BFC-A642-AD14-7BF64597F886}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B21">
+    <sortCondition ref="A1:A21"/>
   </sortState>
-  <tableColumns count="1">
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6A2B8D5C-2437-6844-8856-A6C266ABDCDF}" name="Mechanism"/>
+    <tableColumn id="5" xr3:uid="{61A39BBC-CB40-634D-BC85-71674B0976DC}" name="Equivalent to"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7089,41 +7136,41 @@
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="23" priority="18"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B274">
+    <cfRule type="duplicateValues" dxfId="22" priority="216"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="217"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="218"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B269">
-    <cfRule type="duplicateValues" dxfId="22" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="18" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C270">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
+  <conditionalFormatting sqref="C21:C49 C126:C144 C163:C197">
+    <cfRule type="containsBlanks" dxfId="13" priority="20">
+      <formula>LEN(TRIM(C21))=0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C246">
     <cfRule type="containsBlanks" dxfId="12" priority="13">
       <formula>LEN(TRIM(C246))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C49 C126:C144 C163:C197">
-    <cfRule type="containsBlanks" dxfId="11" priority="20">
-      <formula>LEN(TRIM(C21))=0</formula>
-    </cfRule>
+  <conditionalFormatting sqref="C270">
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D252">
-    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B274">
-    <cfRule type="duplicateValues" dxfId="7" priority="216"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="217"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="218"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="12"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B177" r:id="rId1" tooltip="Difurazone (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Difurazone&amp;action=edit&amp;redlink=1" xr:uid="{E770FD6D-E0C8-2546-98CF-4D2336B593A1}"/>
@@ -7145,64 +7192,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5C6DCB-2CAD-F249-AAAC-65289214B403}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>804</v>
+      </c>
+      <c r="B3" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+        <v>805</v>
+      </c>
+      <c r="B7" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>799</v>
       </c>
     </row>

</xml_diff>